<commit_message>
feat(calendar): Add ics file
</commit_message>
<xml_diff>
--- a/data/Epitech Modules.xlsx/content.xlsx
+++ b/data/Epitech Modules.xlsx/content.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documents\Personal\self-hosted\jsreport\data\Epitech Modules.xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documents\Personal\random\data\Epitech Modules.xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A979AA1-A75F-43AF-99CE-E4DB2F6310EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342CC96C-1F99-42DE-8C2A-B96F798F9BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{60D7B1DA-3E10-411E-A53E-1CC60016F869}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$7:$M$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$7:$N$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Module</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>{{ toC hasProgressiveCredits }}</t>
+  </si>
+  <si>
+    <t>Seats</t>
+  </si>
+  <si>
+    <t>{{ seats }}</t>
   </si>
 </sst>
 </file>
@@ -202,45 +208,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="29">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
     </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
@@ -344,22 +361,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6303C07A-960C-4DFD-B7D5-E029EA2F0F46}" name="Tableau1" displayName="Tableau1" ref="A7:M9" totalsRowCount="1" dataDxfId="26">
-  <autoFilter ref="A7:M8" xr:uid="{D26F5A75-FE85-494B-8332-F8F5FC06450E}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A0906106-458B-4114-9AEA-ADCAD81EDE7B}" name="Module" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{63AB1B13-D226-4459-A5A1-A58DC2270CD3}" name="In Team" dataDxfId="24" totalsRowDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{95E78C62-4558-420C-83DA-389D79E14C67}" name="Team Size" dataDxfId="23" totalsRowDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{05FC7552-AC62-434C-B675-8A8DB993DD5C}" name="In Remote" dataDxfId="22" totalsRowDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{39C0B7DB-C3CD-43CF-A659-1523AF952117}" name="Credits" totalsRowFunction="count" dataDxfId="21" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{5C408DCB-AE53-4F3F-9807-23ED105D4B03}" name="Progressive" dataDxfId="20" totalsRowDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{8E10A061-07E6-4239-9A12-18D01AB1D710}" name="Module/Register start" dataDxfId="19" totalsRowDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{1C051091-5C0D-47E0-9A5E-46D65B905792}" name="Module end" dataDxfId="18" totalsRowDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{D2C14BCB-575F-4051-A0DC-9003849BE0DA}" name="Register end" dataDxfId="17" totalsRowDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{B4BCF7BB-39D9-4366-942F-6557B1F99128}" name="Project Title" dataDxfId="16" totalsRowDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{1EDAB214-8D64-439D-BF5E-B376DC9DE58D}" name="Project start" dataDxfId="15" totalsRowDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{E0C1C683-0EF3-4CC6-8378-5EEE1F305132}" name="Project end" dataDxfId="14" totalsRowDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{3E759C3F-3BFF-433B-B1BE-51BEBBF0CB1F}" name="Link" dataDxfId="13" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6303C07A-960C-4DFD-B7D5-E029EA2F0F46}" name="Tableau1" displayName="Tableau1" ref="A7:N9" totalsRowCount="1" dataDxfId="28">
+  <autoFilter ref="A7:N8" xr:uid="{D26F5A75-FE85-494B-8332-F8F5FC06450E}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{A0906106-458B-4114-9AEA-ADCAD81EDE7B}" name="Module" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{63AB1B13-D226-4459-A5A1-A58DC2270CD3}" name="In Team" dataDxfId="26" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{95E78C62-4558-420C-83DA-389D79E14C67}" name="Team Size" dataDxfId="25" totalsRowDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{05FC7552-AC62-434C-B675-8A8DB993DD5C}" name="In Remote" dataDxfId="24" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{39C0B7DB-C3CD-43CF-A659-1523AF952117}" name="Credits" totalsRowFunction="count" dataDxfId="23" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{5C408DCB-AE53-4F3F-9807-23ED105D4B03}" name="Progressive" dataDxfId="22" totalsRowDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{705BE21A-48B7-4E15-8452-73360A29AAD1}" name="Seats" dataDxfId="14" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{8E10A061-07E6-4239-9A12-18D01AB1D710}" name="Module/Register start" dataDxfId="21" totalsRowDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{1C051091-5C0D-47E0-9A5E-46D65B905792}" name="Module end" dataDxfId="20" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{D2C14BCB-575F-4051-A0DC-9003849BE0DA}" name="Register end" dataDxfId="19" totalsRowDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{B4BCF7BB-39D9-4366-942F-6557B1F99128}" name="Project Title" dataDxfId="18" totalsRowDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{1EDAB214-8D64-439D-BF5E-B376DC9DE58D}" name="Project start" dataDxfId="17" totalsRowDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{E0C1C683-0EF3-4CC6-8378-5EEE1F305132}" name="Project end" dataDxfId="16" totalsRowDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{3E759C3F-3BFF-433B-B1BE-51BEBBF0CB1F}" name="Link" dataDxfId="15" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -683,10 +701,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26F5A75-FE85-494B-8332-F8F5FC06450E}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,14 +712,14 @@
     <col min="1" max="1" width="60.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="4" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="60.7109375" customWidth="1"/>
-    <col min="11" max="12" width="25.7109375" customWidth="1"/>
-    <col min="13" max="13" width="60.7109375" customWidth="1"/>
+    <col min="6" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="60.7109375" customWidth="1"/>
+    <col min="12" max="13" width="25.7109375" customWidth="1"/>
+    <col min="14" max="14" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -709,7 +727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -720,7 +738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -740,28 +758,31 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>14</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>3</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>19</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>7</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>8</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -780,29 +801,32 @@
       <c r="F8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="L8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="M8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="N8" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -821,6 +845,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>